<commit_message>
Correcciones que hizo el profe
Modifique y agregue unos casos de prueba, ya que el profe nos dio una correccion
</commit_message>
<xml_diff>
--- a/tests_cases/TC-Print2-01.xlsx
+++ b/tests_cases/TC-Print2-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igu/Documents/UADE/Testing de aplicacioones /TestingAplicaciones-TPO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\GitHub\TestingAplicaciones--Jarron-Shang--TPO\tests_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E09EA65-4B5D-2D43-9DBE-62FE5F79B57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA513C7F-71D7-4151-A96A-9C3766B297DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="760" windowWidth="14660" windowHeight="17640" xr2:uid="{D25F4DC2-856B-BD4F-8D8D-2077668DD2F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D25F4DC2-856B-BD4F-8D8D-2077668DD2F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Expected Results</t>
   </si>
   <si>
-    <t>TC-Print 2-01</t>
-  </si>
-  <si>
     <t>Test del Log in</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Acceso a la pagina de compra</t>
   </si>
   <si>
-    <t>Userid = test@mail.com</t>
-  </si>
-  <si>
     <t>No aplicada</t>
   </si>
   <si>
@@ -125,24 +119,15 @@
     <t>Se deberia poder logear si y solo si los datos son correctos</t>
   </si>
   <si>
-    <t>Pass = password1232</t>
-  </si>
-  <si>
     <t>User id = test@email.com</t>
   </si>
   <si>
     <t>El usuario deberia tener cuenta</t>
   </si>
   <si>
-    <t>URL: quierocomprar.com</t>
-  </si>
-  <si>
     <t>Abrir un navegador web : Google Chrome</t>
   </si>
   <si>
-    <t>Ingresar a la pagina quierocomprar.com</t>
-  </si>
-  <si>
     <t>Se deberia entrar a la pagina deseada</t>
   </si>
   <si>
@@ -155,28 +140,16 @@
     <t>Se deberia ingresar a la pagina con la cuenta del usuario</t>
   </si>
   <si>
-    <t>Camino alternativo</t>
-  </si>
-  <si>
-    <t>Se deberia mostar en pantalla un cartel de error</t>
-  </si>
-  <si>
-    <t>Intenta de nuevo con los mismo datos</t>
-  </si>
-  <si>
-    <t>Se deberia mostar en pantalla un cartel de usuario bloqueado</t>
-  </si>
-  <si>
-    <t>Ingresa mail en el formulario para blanquear password</t>
-  </si>
-  <si>
-    <t>Se deberia mandar al mail, el password</t>
-  </si>
-  <si>
-    <t>Abrir un navegador web : FireFox</t>
-  </si>
-  <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>TC-Print 2-03</t>
+  </si>
+  <si>
+    <t>Ingresar a la pagina http://127.0.0.1:5000</t>
+  </si>
+  <si>
+    <t>URL: http://127.0.0.1:5000</t>
   </si>
 </sst>
 </file>
@@ -486,7 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -500,9 +473,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -519,9 +489,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -535,9 +502,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,18 +522,69 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -583,68 +598,17 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -965,395 +929,232 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="37"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D1" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="15">
+        <v>2</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>3</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="51"/>
+      <c r="D10" s="15">
+        <v>3</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+    </row>
+    <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="47"/>
+    </row>
+    <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>1</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>2</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
         <v>4</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
-        <v>1</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="18">
-        <v>1</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
-        <v>2</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="18">
-        <v>2</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
-        <v>3</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="18">
-        <v>3</v>
-      </c>
-      <c r="E10" s="17" t="s">
+      <c r="B22" s="28" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-    </row>
-    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="33"/>
-    </row>
-    <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24">
-        <v>1</v>
-      </c>
-      <c r="B19" s="34" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24">
-        <v>2</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24">
-        <v>3</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24">
-        <v>4</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="51"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
-        <v>1</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="18">
-        <v>1</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
-        <v>2</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="18">
-        <v>2</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D30" s="18">
-        <v>3</v>
-      </c>
-      <c r="E30" s="17"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="33"/>
-    </row>
-    <row r="33" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24">
-        <v>1</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="35"/>
-    </row>
-    <row r="34" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="24">
-        <v>2</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="35"/>
-    </row>
-    <row r="35" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24">
-        <v>3</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="35"/>
-    </row>
-    <row r="36" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24">
-        <v>4</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="35"/>
-    </row>
-    <row r="37" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29">
-        <v>5</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="35"/>
-    </row>
-    <row r="38" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24">
-        <v>6</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="51"/>
-    </row>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="33" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
+  <mergeCells count="15">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:E15"/>
@@ -1361,22 +1162,12 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D35:E35"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B33:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
executions hechos y registrados
Hice los executions de los casos de prueba con priority High
</commit_message>
<xml_diff>
--- a/tests_cases/TC-Print2-01.xlsx
+++ b/tests_cases/TC-Print2-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\GitHub\TestingAplicaciones--Jarron-Shang--TPO\tests_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97D4A50-32D7-4A61-B230-23E3359DC1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20244B45-2E62-44DD-8B54-36214E6CE58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D25F4DC2-856B-BD4F-8D8D-2077668DD2F1}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>Regression 1</t>
   </si>
   <si>
-    <t>Tester: Sam Peters</t>
-  </si>
-  <si>
     <t>Actual Results</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Ingresar datos de usuario:sample@example.com y pass: sample</t>
+  </si>
+  <si>
+    <t>Tester: Ignacio Tsai</t>
   </si>
 </sst>
 </file>
@@ -197,6 +197,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -688,81 +689,84 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,9 +775,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1107,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D36A19-2677-574C-8EC2-0AD18FFA1610}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1208,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1303,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="51" t="s">
@@ -1326,32 +1327,32 @@
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
     </row>
     <row r="26" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="55"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B27" s="58"/>
       <c r="C27" s="58"/>
@@ -1363,59 +1364,59 @@
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="60"/>
       <c r="C28" s="60"/>
       <c r="D28" s="60"/>
       <c r="E28" s="60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="60"/>
       <c r="G28" s="60"/>
       <c r="H28" s="60"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="33" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1425,6 +1426,16 @@
     <row r="38" ht="30.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
@@ -1441,16 +1452,6 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>